<commit_message>
Implementação para carregar um arquivo de regra especifico dependendo do tipo definido: XLSX OU DRL, parâmetro definido na requisição
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/planilhas/customer-rules.xlsx
+++ b/src/main/resources/rules/planilhas/customer-rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto Motor de Regras com drools\spring-boot-drools-example\src\main\resources\rules\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09E2E52-37A5-453C-BBF4-9D703C250D6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FB9B82-AA3F-4B63-8B5A-BD2A9218FD20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -658,7 +658,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="1">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>